<commit_message>
Moved keyboard buffer (in memory map)
</commit_message>
<xml_diff>
--- a/memory_map.xlsx
+++ b/memory_map.xlsx
@@ -20,11 +20,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t xml:space="preserve">All Values are in HEXADECIMAL notation</t>
   </si>
   <si>
+    <t xml:space="preserve">BOLD:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Free Memory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Underline:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memory occupied by x86 PC Stuff</t>
+  </si>
+  <si>
     <t xml:space="preserve">Address</t>
   </si>
   <si>
@@ -52,9 +64,6 @@
     <t xml:space="preserve">True</t>
   </si>
   <si>
-    <t xml:space="preserve">Free Memory</t>
-  </si>
-  <si>
     <t xml:space="preserve">False</t>
   </si>
   <si>
@@ -67,16 +76,16 @@
     <t xml:space="preserve">BA00</t>
   </si>
   <si>
+    <t xml:space="preserve">Keyboard Buffer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n.a. (from KERNEL)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Shell Code and Static Data</t>
   </si>
   <si>
     <t xml:space="preserve">SHELL.RNB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keyboard Buffer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n.a. (from SHELL)</t>
   </si>
   <si>
     <t xml:space="preserve">EBDA</t>
@@ -93,11 +102,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="14">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+  <fonts count="17">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -115,63 +125,99 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b val="true"/>
+      <sz val="24"/>
       <color rgb="FF000000"/>
-      <name val="Noto Sans Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Noto Sans Devanagari"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
-      <name val="Noto Sans Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
       <sz val="10"/>
       <color rgb="FF808080"/>
-      <name val="Noto Sans Devanagari"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF006600"/>
-      <name val="Noto Sans Devanagari"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
-      <name val="Noto Sans Devanagari"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFCC0000"/>
-      <name val="Noto Sans Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Noto Sans Devanagari"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="11">
@@ -306,32 +352,72 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -344,15 +430,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -449,17 +527,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.14"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
@@ -471,228 +549,244 @@
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="B4" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="str">
+      <c r="C7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="str">
         <f aca="false">T("7C00")</f>
         <v>7C00</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="0" t="str">
+      <c r="B8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="0" t="str">
         <f aca="false">T("200")</f>
         <v>200</v>
       </c>
-      <c r="F3" s="0" t="str">
+      <c r="F8" s="0" t="str">
         <f aca="false">T("7E00")</f>
         <v>7E00</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="str">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="str">
         <f aca="false">T("7E00")</f>
         <v>7E00</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="0" t="str">
+      <c r="B9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="0" t="str">
         <f aca="false">T("1000")</f>
         <v>1000</v>
       </c>
-      <c r="F4" s="0" t="str">
+      <c r="F9" s="0" t="str">
         <f aca="false">T("8E00")</f>
         <v>8E00</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="str">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="str">
         <f aca="false">T("8E00")</f>
         <v>8E00</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="0" t="s">
+      <c r="B10" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="0" t="str">
+      <c r="E10" s="0" t="str">
         <f aca="false">T("4400")</f>
         <v>4400</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="str">
+      <c r="F10" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="str">
         <f aca="false">T("BA00")</f>
         <v>BA00</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="0" t="str">
-        <f aca="false">DEC2HEX(HEX2DEC(F6) - HEX2DEC(A6), 10)</f>
-        <v>0000004600</v>
-      </c>
-      <c r="F6" s="0" t="str">
+      <c r="B11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="0" t="str">
+        <f aca="false">T("400")</f>
+        <v>400</v>
+      </c>
+      <c r="F11" s="0" t="str">
+        <f aca="false">DEC2HEX((HEX2DEC(A11)+HEX2DEC(E11)), 10)</f>
+        <v>000000BE00</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="str">
+        <f aca="false">T("BE00")</f>
+        <v>BE00</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="0" t="str">
+        <f aca="false">DEC2HEX(HEX2DEC(F12) - HEX2DEC(A12), 10)</f>
+        <v>0000004200</v>
+      </c>
+      <c r="F12" s="0" t="str">
         <f aca="false">T("10000")</f>
         <v>10000</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="str">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="str">
         <f aca="false">T("10000")</f>
         <v>10000</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="0" t="str">
+      <c r="B13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="0" t="str">
         <f aca="false">T("E00")</f>
         <v>E00</v>
       </c>
-      <c r="F7" s="0" t="str">
-        <f aca="false">DEC2HEX((HEX2DEC(A7)+HEX2DEC(E7)),10)</f>
+      <c r="F13" s="0" t="str">
+        <f aca="false">DEC2HEX((HEX2DEC(A13)+HEX2DEC(E13)),10)</f>
         <v>0000010E00</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="str">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="str">
         <f aca="false">T("10E00")</f>
         <v>10E00</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="0" t="str">
-        <f aca="false">T("400")</f>
-        <v>400</v>
-      </c>
-      <c r="F8" s="0" t="str">
-        <f aca="false">DEC2HEX((HEX2DEC(A8)+HEX2DEC(E8)), 10)</f>
-        <v>0000011200</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="str">
-        <f aca="false">T("11200")</f>
-        <v>11200</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="0" t="str">
-        <f aca="false">DEC2HEX(HEX2DEC(F9)-HEX2DEC(A9),10)</f>
-        <v>000008EA00</v>
-      </c>
-      <c r="F9" s="0" t="str">
+      <c r="B14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="0" t="str">
+        <f aca="false">DEC2HEX(HEX2DEC(F14)-HEX2DEC(A14),10)</f>
+        <v>000008EE00</v>
+      </c>
+      <c r="F14" s="0" t="str">
         <f aca="false">T("9FC00")</f>
         <v>9FC00</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="str">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="str">
         <f aca="false">T("9FC00")</f>
         <v>9FC00</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="0" t="str">
-        <f aca="false">DEC2HEX(HEX2DEC(F10)-HEX2DEC(A10),10)</f>
+      <c r="B15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="0" t="str">
+        <f aca="false">DEC2HEX(HEX2DEC(F15)-HEX2DEC(A15),10)</f>
         <v>0000000400</v>
       </c>
-      <c r="F10" s="0" t="str">
+      <c r="F15" s="0" t="str">
         <f aca="false">T("A0000")</f>
         <v>A0000</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="str">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="str">
         <f aca="false">T("A0000")</f>
         <v>A0000</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="0" t="str">
-        <f aca="false">DEC2HEX(HEX2DEC(F11)-HEX2DEC(A11),10)</f>
+      <c r="B16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="0" t="str">
+        <f aca="false">DEC2HEX(HEX2DEC(F16)-HEX2DEC(A16),10)</f>
         <v>0000060000</v>
       </c>
-      <c r="F11" s="0" t="str">
+      <c r="F16" s="0" t="str">
         <f aca="false">T("100000")</f>
         <v>100000</v>
       </c>

</xml_diff>

<commit_message>
Added keyboard buffer Added basic shell functionaltity Added new functions to libkernel Added macro to libkernel for quick use of INT49
</commit_message>
<xml_diff>
--- a/memory_map.xlsx
+++ b/memory_map.xlsx
@@ -530,14 +530,14 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.14"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>

</xml_diff>

<commit_message>
Added first pass of ELF definitions
</commit_message>
<xml_diff>
--- a/memory_map.xlsx
+++ b/memory_map.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t xml:space="preserve">All Values are in HEXADECIMAL notation</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t xml:space="preserve">SHELL.RNB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELF file loader</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELFL.RNB</t>
   </si>
   <si>
     <t xml:space="preserve">EBDA</t>
@@ -102,7 +108,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -219,8 +225,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -279,6 +290,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF7F00"/>
         <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF007FFF"/>
+        <bgColor rgb="FF3366FF"/>
       </patternFill>
     </fill>
   </fills>
@@ -401,7 +418,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -430,7 +447,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -483,7 +512,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FF007FFF"/>
       <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF0000A8"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -527,10 +556,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -609,24 +638,24 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="str">
+      <c r="A9" s="7" t="str">
         <f aca="false">T("7E00")</f>
         <v>7E00</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="0" t="str">
+      <c r="E9" s="7" t="str">
         <f aca="false">T("1000")</f>
         <v>1000</v>
       </c>
-      <c r="F9" s="0" t="str">
+      <c r="F9" s="7" t="str">
         <f aca="false">T("8E00")</f>
         <v>8E00</v>
       </c>
@@ -677,24 +706,24 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="str">
+      <c r="A12" s="7" t="str">
         <f aca="false">T("BE00")</f>
         <v>BE00</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="0" t="str">
+      <c r="E12" s="7" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(F12) - HEX2DEC(A12), 10)</f>
         <v>0000004200</v>
       </c>
-      <c r="F12" s="0" t="str">
+      <c r="F12" s="7" t="str">
         <f aca="false">T("10000")</f>
         <v>10000</v>
       </c>
@@ -714,79 +743,102 @@
         <v>13</v>
       </c>
       <c r="E13" s="0" t="str">
-        <f aca="false">T("E00")</f>
-        <v>E00</v>
+        <f aca="false">T("1C00")</f>
+        <v>1C00</v>
       </c>
       <c r="F13" s="0" t="str">
         <f aca="false">DEC2HEX((HEX2DEC(A13)+HEX2DEC(E13)),10)</f>
-        <v>0000010E00</v>
+        <v>0000011C00</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="str">
-        <f aca="false">T("10E00")</f>
-        <v>10E00</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="A14" s="0" t="str">
+        <f aca="false">F13</f>
+        <v>0000011C00</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="0" t="str">
+        <f aca="false">T("1C00")</f>
+        <v>1C00</v>
+      </c>
+      <c r="F14" s="9" t="str">
+        <f aca="false">DEC2HEX((HEX2DEC(A14)+HEX2DEC(E14)),10)</f>
+        <v>0000013800</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10" t="str">
+        <f aca="false">F14</f>
+        <v>0000013800</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="0" t="str">
-        <f aca="false">DEC2HEX(HEX2DEC(F14)-HEX2DEC(A14),10)</f>
-        <v>000008EE00</v>
-      </c>
-      <c r="F14" s="0" t="str">
+      <c r="E15" s="7" t="str">
+        <f aca="false">DEC2HEX(HEX2DEC(F15)-HEX2DEC(A15),10)</f>
+        <v>000008C400</v>
+      </c>
+      <c r="F15" s="7" t="str">
         <f aca="false">T("9FC00")</f>
         <v>9FC00</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="str">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="str">
         <f aca="false">T("9FC00")</f>
         <v>9FC00</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="0" t="s">
+      <c r="B16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D16" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="0" t="str">
-        <f aca="false">DEC2HEX(HEX2DEC(F15)-HEX2DEC(A15),10)</f>
+      <c r="E16" s="0" t="str">
+        <f aca="false">DEC2HEX(HEX2DEC(F16)-HEX2DEC(A16),10)</f>
         <v>0000000400</v>
       </c>
-      <c r="F15" s="0" t="str">
+      <c r="F16" s="0" t="str">
         <f aca="false">T("A0000")</f>
         <v>A0000</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="str">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="str">
         <f aca="false">T("A0000")</f>
         <v>A0000</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="0" t="s">
+      <c r="B17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D17" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="0" t="str">
-        <f aca="false">DEC2HEX(HEX2DEC(F16)-HEX2DEC(A16),10)</f>
+      <c r="E17" s="0" t="str">
+        <f aca="false">DEC2HEX(HEX2DEC(F17)-HEX2DEC(A17),10)</f>
         <v>0000060000</v>
       </c>
-      <c r="F16" s="0" t="str">
+      <c r="F17" s="0" t="str">
         <f aca="false">T("100000")</f>
         <v>100000</v>
       </c>

</xml_diff>